<commit_message>
updated data quality scores
</commit_message>
<xml_diff>
--- a/scoring_table.xlsx
+++ b/scoring_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruben/PycharmProjects/mitre_attack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/PycharmProjects/Blue-ATTACK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2CE29A-4C0A-7147-921A-373F057A25D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4438F7AF-659C-6441-93E6-12D9ACD22FBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37500" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="27900" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detection scores - descriptions" sheetId="1" r:id="rId1"/>
@@ -327,28 +327,7 @@
     <t>5 - Excellent</t>
   </si>
   <si>
-    <t>Data source is available for 100% of the devices.
-Data is retained for 100% of the required time.</t>
-  </si>
-  <si>
     <t>Retention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data source is available from 
-0-25% of the devices.
-Data is retained 0-25% of the required time. </t>
-  </si>
-  <si>
-    <t>Data source is available from 26-50% of the devices.
-Data is retained 26-50% of the required time.</t>
-  </si>
-  <si>
-    <t>Data source is available from 51-75% of the devices.
-Data is retained 51-75% of the required time.</t>
-  </si>
-  <si>
-    <t>Data source is available from 76-100% of the devices.
-Data is retained 76-99% of the required time.</t>
   </si>
   <si>
     <t>Required fields are available from 76-99%.</t>
@@ -398,6 +377,23 @@
   </si>
   <si>
     <t>Data is stored for 30 days, but we ideally want to have it for 1 year.</t>
+  </si>
+  <si>
+    <t>Data source is available from 
+0-25% of the devices.</t>
+  </si>
+  <si>
+    <t>Data source is available from 26-50% of the devices.</t>
+  </si>
+  <si>
+    <t>Data source is available from 51-75% of the devices.</t>
+  </si>
+  <si>
+    <t>Data source is available from 76-100% of the devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data source is available for 100% of the devices.
+</t>
   </si>
 </sst>
 </file>
@@ -1415,7 +1411,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1676,7 +1672,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>28</v>
@@ -1836,7 +1832,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33.75" customHeight="1">
@@ -2012,7 +2008,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>54</v>
@@ -2065,16 +2061,16 @@
     </row>
     <row r="7" spans="1:4" ht="86" thickBot="1">
       <c r="A7" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
@@ -2122,7 +2120,7 @@
         <v>63</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34">
@@ -2150,7 +2148,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>71</v>
@@ -2162,23 +2160,23 @@
         <v>72</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="85">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34">
       <c r="A5" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="52"/>
       <c r="F5" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136">
@@ -2186,35 +2184,35 @@
         <v>76</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="85">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34">
       <c r="A7" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="52"/>
       <c r="F7" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86" thickBot="1">
@@ -2222,7 +2220,7 @@
         <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>80</v>
@@ -2234,7 +2232,7 @@
         <v>78</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2292,6 +2290,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008848E62C5F483F46BBC45A037BA06456" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9a231ef8203bd2df6f980a33ee7564c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="647e26e098842d3908dd56dced403b39" ns2:_="">
     <xsd:import namespace="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
@@ -2437,15 +2444,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
   <ds:schemaRefs>
@@ -2463,6 +2461,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3CD046-562E-4048-8CB3-7B082ACE1CD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2478,12 +2484,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrections/improvements on the data quality, visibility and detection scores.
</commit_message>
<xml_diff>
--- a/scoring_table.xlsx
+++ b/scoring_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/PycharmProjects/Blue-ATTACK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D100A5AA-3602-814C-9095-C471334553F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF13A30-7F5A-DA41-9E82-7B9D3CF8A7FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detection scores - descriptions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
   <si>
     <t>Detection scores</t>
   </si>
@@ -107,9 +107,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Possibly not realtime</t>
-  </si>
-  <si>
     <t>Signature based</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>More complex analytics</t>
   </si>
   <si>
-    <t>Realtime</t>
-  </si>
-  <si>
     <t>Many known aspects of the technique</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>Almost all known aspects of the technique</t>
   </si>
   <si>
-    <t>Bypassing (evarion/obfuscation) is hard</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -173,18 +164,9 @@
     <t>Minimal</t>
   </si>
   <si>
-    <t>Sufficient data sources available to be able to see one aspect of the technique's procedures.</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Sufficient data sources available to be able to see almost all known aspects of the technique's procedures.</t>
-  </si>
-  <si>
-    <t>All data sources necessary to be able to see all known aspects of the technique's procedures are available.</t>
-  </si>
-  <si>
     <t>Questions?</t>
   </si>
   <si>
@@ -194,10 +176,6 @@
     <t>Device completeness</t>
   </si>
   <si>
-    <t>When doing an hunting investigation can we cover all devices/users that we need to?
-For how long is the data available?</t>
-  </si>
-  <si>
     <t>Data completeness</t>
   </si>
   <si>
@@ -207,193 +185,217 @@
     <t>Are all the required data fields in the event present to perform my investigation?</t>
   </si>
   <si>
-    <t>We have proxy logs, but they the logs do not contain the "Host" header.</t>
-  </si>
-  <si>
     <t>Timeliness</t>
   </si>
   <si>
     <t xml:space="preserve">Indicates when data is available, and how accurate the timestamps of the data are in relation to the actual time an event occurred. </t>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Says something about the standardisation of data field names and types. </t>
+  </si>
+  <si>
+    <t>Can we correlate the events with other data sources?
+Can we run queries across all data sources using standard naming conventions for specific fields?</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Data quality - dimensions</t>
+  </si>
+  <si>
+    <t>Data field completeness</t>
+  </si>
+  <si>
+    <t>0 - None</t>
+  </si>
+  <si>
+    <t>1 - Poor</t>
+  </si>
+  <si>
+    <t>2 - Fair</t>
+  </si>
+  <si>
+    <t>3 - Good</t>
+  </si>
+  <si>
+    <t>4 - Very good</t>
+  </si>
+  <si>
+    <t>100% of the fields is standardized in name and type.</t>
+  </si>
+  <si>
+    <t>The data is available right away.
+The timestamps in the data are 100% accurate.</t>
+  </si>
+  <si>
+    <t>Required fields are available for 100%.</t>
+  </si>
+  <si>
+    <t>It takes a while before the data is available, but is acceptable.
+The timestamps in the data have a small deviation with the actual time events occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It takes a long time before the data is available.
+The timestamps in the data deviate much from the actual time events occurred. </t>
+  </si>
+  <si>
+    <t>76-99%</t>
+  </si>
+  <si>
+    <t>51-75%</t>
+  </si>
+  <si>
+    <t>26-50%</t>
+  </si>
+  <si>
+    <t>No data sources</t>
+  </si>
+  <si>
+    <t>26-50% of data sources available</t>
+  </si>
+  <si>
+    <t>51-75% of data sources available</t>
+  </si>
+  <si>
+    <t>76-99% of data sources available</t>
+  </si>
+  <si>
+    <t>100% of data sources available</t>
+  </si>
+  <si>
+    <t>Data sources - legend</t>
+  </si>
+  <si>
+    <t>Do not know / not documented / not applicable</t>
+  </si>
+  <si>
+    <t>5 - Excellent</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>Required fields are available from 76-99%.</t>
+  </si>
+  <si>
+    <t>Required fields are available from 51-75%.</t>
+  </si>
+  <si>
+    <t>Required fields are available from 26-50%.</t>
+  </si>
+  <si>
+    <t>51-99% of the fields is standardized in name and type.</t>
+  </si>
+  <si>
+    <t>Data is stored for 100% of the desired retention period.</t>
+  </si>
+  <si>
+    <t>Data retention is within 
+51-75% of the desired period.</t>
+  </si>
+  <si>
+    <t>Data retention is within 
+76-99% of the desired period.</t>
+  </si>
+  <si>
+    <t>Data retention is within 
+26-50% of the desired period.</t>
+  </si>
+  <si>
+    <t>More aspects of the technique compared to "1/Basic"</t>
+  </si>
+  <si>
+    <t>Data is stored for 30 days, but we ideally want to have it for 1 year.</t>
+  </si>
+  <si>
+    <t>Data source is available from 26-50% of the devices.</t>
+  </si>
+  <si>
+    <t>Data source is available from 51-75% of the devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data source is available for 100% of the devices.
+</t>
+  </si>
+  <si>
+    <t>Data source is available from 76-99% of the devices.</t>
+  </si>
+  <si>
+    <t>Possibly not real time</t>
+  </si>
+  <si>
+    <t>Bypassing (evasion/obfuscation) is hard</t>
+  </si>
+  <si>
+    <t>Real time</t>
+  </si>
+  <si>
+    <t>Indicates how long the data is stored compared to the desired data retention period.</t>
+  </si>
+  <si>
+    <t>Indicates if the required data is available for all involved devices.</t>
+  </si>
+  <si>
+    <t>When doing a hunting investigation can we cover all devices/users that we need to?</t>
+  </si>
+  <si>
+    <t>For how long is the data available?
+How long do you want to keep the data?</t>
+  </si>
+  <si>
+    <t>We are missing event data for endpoints running an older version of Windows.</t>
+  </si>
+  <si>
+    <t>We have proxy logs, but the events do not contain the "Host" header.</t>
+  </si>
+  <si>
+    <t>We have a delay of 1-2 days to get the necessary data from all endpoints into the security data lake.
+Timestamps are representing not the time an event occurred, but ingestion time in the security data lake.</t>
   </si>
   <si>
     <t>Is the data available right away when we need it?
 Do the timestamps in the data represent the time the record was created or ingested?</t>
   </si>
   <si>
-    <t>We have a delay of 1-2 day to get the necessary data from all endpoints into the security data lake.
-Timestamps are representing not the time an event occurred, but ingestion time in the security data lake.</t>
-  </si>
-  <si>
-    <t>Consistency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Says something about the standardisation of data field names and types. </t>
-  </si>
-  <si>
-    <t>Can we correlate the events with other data sources?
-Can we run queries across all data sources using standard naming conventions for specific fields?</t>
-  </si>
-  <si>
-    <t>Fields within events across different data sources do not have the same name.</t>
-  </si>
-  <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
-    <t>Data quality - dimensions</t>
-  </si>
-  <si>
-    <t>Data quality - scoring</t>
-  </si>
-  <si>
-    <t>Data field completeness</t>
-  </si>
-  <si>
-    <t>Required fields are available from 0-25%.</t>
-  </si>
-  <si>
-    <t>0-50% of the fields is standardized in name and type.</t>
-  </si>
-  <si>
-    <t>0 - None</t>
-  </si>
-  <si>
-    <t>1 - Poor</t>
-  </si>
-  <si>
-    <t>2 - Fair</t>
-  </si>
-  <si>
-    <t>3 - Good</t>
-  </si>
-  <si>
-    <t>4 - Very good</t>
-  </si>
-  <si>
-    <t>100% of the fields is standardized in name and type.</t>
-  </si>
-  <si>
-    <t>The data is available right away.
-The timestamps in the data are 100% accurate.</t>
-  </si>
-  <si>
-    <t>Required fields are available for 100%.</t>
-  </si>
-  <si>
-    <t>It takes a while before the data is available, but is acceptable.
-The timestamps in the data have a small deviation with the actual time events occurred.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It takes a long time before the data is available.
-The timestamps in the data deviate much from the actual time events occurred. </t>
-  </si>
-  <si>
-    <t>76-99%</t>
-  </si>
-  <si>
-    <t>51-75%</t>
-  </si>
-  <si>
-    <t>26-50%</t>
-  </si>
-  <si>
-    <t>0-25%</t>
-  </si>
-  <si>
-    <t>No data sources</t>
-  </si>
-  <si>
-    <t>0-25% of data sources available</t>
-  </si>
-  <si>
-    <t>26-50% of data sources available</t>
-  </si>
-  <si>
-    <t>51-75% of data sources available</t>
-  </si>
-  <si>
-    <t>76-99% of data sources available</t>
-  </si>
-  <si>
-    <t>100% of data sources available</t>
-  </si>
-  <si>
-    <t>Data sources - legend</t>
-  </si>
-  <si>
-    <t>Do not know / not documented / not applicable</t>
-  </si>
-  <si>
-    <t>5 - Excellent</t>
-  </si>
-  <si>
-    <t>Retention</t>
-  </si>
-  <si>
-    <t>Required fields are available from 76-99%.</t>
-  </si>
-  <si>
-    <t>Required fields are available from 51-75%.</t>
-  </si>
-  <si>
-    <t>Required fields are available from 26-50%.</t>
-  </si>
-  <si>
-    <t>51-99% of the fields is standardized in name and type.</t>
-  </si>
-  <si>
-    <t>Data retention is within 0-25% of the desired period.</t>
-  </si>
-  <si>
-    <t>Data is stored for 100% of the desired retention period.</t>
-  </si>
-  <si>
-    <t>Data retention is within 
-51-75% of the desired period.</t>
-  </si>
-  <si>
-    <t>Data retention is within 
-76-99% of the desired period.</t>
-  </si>
-  <si>
-    <t>Data retention is within 
-26-50% of the desired period.</t>
-  </si>
-  <si>
-    <t>More aspects of the technique compared to "1/Basic"</t>
-  </si>
-  <si>
-    <t>Sufficient data sources available to be able to see more aspects of the technique's procedures compared to "1/Minimal".</t>
-  </si>
-  <si>
-    <t>Indicates if required data is available for all involved devices and indicates how the data is retained compared to the desired data retention.</t>
-  </si>
-  <si>
-    <t>Indicates how long data is stored and thus available for your blue team.</t>
-  </si>
-  <si>
-    <t>How long is the data stored and available?
-How long do you want to keep the data?</t>
-  </si>
-  <si>
-    <t>Data is stored for 30 days, but we ideally want to have it for 1 year.</t>
+    <t>Field names within this data source are not in line with that of other data sources.</t>
+  </si>
+  <si>
+    <t>Data quality - scores</t>
+  </si>
+  <si>
+    <t>1-25% of data sources available</t>
+  </si>
+  <si>
+    <t>1-25%</t>
   </si>
   <si>
     <t>Data source is available from 
-0-25% of the devices.</t>
-  </si>
-  <si>
-    <t>Data source is available from 26-50% of the devices.</t>
-  </si>
-  <si>
-    <t>Data source is available from 51-75% of the devices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data source is available for 100% of the devices.
-</t>
-  </si>
-  <si>
-    <t>Data source is available from 76-99% of the devices.</t>
+1-25% of the devices.</t>
+  </si>
+  <si>
+    <t>Required fields are available from 1-25%.</t>
+  </si>
+  <si>
+    <t>1-50% of the fields is standardized in name and type.</t>
+  </si>
+  <si>
+    <t>Data retention is within 1-25% of the desired period.</t>
+  </si>
+  <si>
+    <t>All data sources and required data quality necessary to be able to see all known aspects of the technique's procedures are available.</t>
+  </si>
+  <si>
+    <t>Sufficient data sources with sufficient quality available to be able to see almost all known aspects of the technique's procedures.</t>
+  </si>
+  <si>
+    <t>Sufficient data sources with sufficient quality available to be able to see one aspect of the technique's procedures.</t>
+  </si>
+  <si>
+    <t>Sufficient data sources with sufficient quality available to be able to see more aspects of the technique's procedures compared to "1/Minimal".</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1413,9 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1460,7 +1464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="98" customHeight="1">
+    <row r="5" spans="1:3" ht="119">
       <c r="A5" s="15">
         <v>1</v>
       </c>
@@ -1471,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="96.75" customHeight="1">
+    <row r="6" spans="1:3" ht="104" customHeight="1">
       <c r="A6" s="15">
         <v>2</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="65.25" customHeight="1" thickBot="1">
+    <row r="9" spans="1:3" ht="69" customHeight="1" thickBot="1">
       <c r="A9" s="16">
         <v>5</v>
       </c>
@@ -1528,7 +1532,9 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1617,7 +1623,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
@@ -1640,22 +1646,22 @@
         <v>8</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34">
@@ -1666,22 +1672,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34">
@@ -1692,22 +1698,22 @@
         <v>12</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="F7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="H7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34">
@@ -1718,22 +1724,22 @@
         <v>14</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="35" thickBot="1">
@@ -1744,22 +1750,22 @@
         <v>16</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="H9" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1780,9 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1787,7 +1795,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -1810,18 +1818,18 @@
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="33.75" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51">
       <c r="A4" s="15">
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51">
@@ -1829,13 +1837,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="33.75" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51">
       <c r="A6" s="15">
         <v>3</v>
       </c>
@@ -1843,10 +1851,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="35" thickBot="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="52" thickBot="1">
       <c r="A7" s="16">
         <v>4</v>
       </c>
@@ -1854,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1870,7 +1878,9 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1883,7 +1893,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -1906,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="33.75" customHeight="1">
@@ -1914,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17">
@@ -1925,10 +1935,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33.75" customHeight="1">
@@ -1936,19 +1946,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="33.75" customHeight="1">
       <c r="A7" s="42"/>
       <c r="B7" s="47" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" thickBot="1">
@@ -1959,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1971,7 +1981,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -1984,93 +1996,93 @@
   <sheetData>
     <row r="1" spans="1:4" s="22" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="119">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="68">
       <c r="A3" s="28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51">
       <c r="A4" s="28" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="153">
       <c r="A5" s="28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119">
       <c r="A6" s="55" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86" thickBot="1">
       <c r="A7" s="58" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2083,7 +2095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2096,7 +2108,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -2108,131 +2120,131 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="54" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34">
       <c r="A3" s="34" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="102">
       <c r="A4" s="35" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>72</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34">
       <c r="A5" s="35" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="52"/>
       <c r="F5" s="10" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136">
       <c r="A6" s="35" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34">
       <c r="A7" s="35" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="52"/>
       <c r="F7" s="10" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86" thickBot="1">
       <c r="A8" s="36" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2285,6 +2297,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008848E62C5F483F46BBC45A037BA06456" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9a231ef8203bd2df6f980a33ee7564c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="647e26e098842d3908dd56dced403b39" ns2:_="">
     <xsd:import namespace="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
@@ -2430,7 +2448,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2439,13 +2457,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3CD046-562E-4048-8CB3-7B082ACE1CD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2463,26 +2491,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Renamed "Data completeness" to "Data field completeness"
</commit_message>
<xml_diff>
--- a/scoring_table.xlsx
+++ b/scoring_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/PycharmProjects/DeTTACT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/PycharmProjects/DeTTECT-private/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D28C989-ADDE-7F47-B009-8ABB59425DA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E722A-9C3E-5049-BD71-FEA725D581E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detection scores - descriptions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
   <si>
     <t>Detection scores</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Device completeness</t>
-  </si>
-  <si>
-    <t>Data completeness</t>
   </si>
   <si>
     <t>Indicates to what degree the data has the required information/fields.</t>
@@ -1472,7 +1469,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="104" customHeight="1">
@@ -1623,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
@@ -1649,7 +1646,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>25</v>
@@ -1675,10 +1672,10 @@
         <v>29</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>26</v>
@@ -1701,7 +1698,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>33</v>
@@ -1727,13 +1724,13 @@
         <v>32</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>37</v>
@@ -1753,13 +1750,13 @@
         <v>32</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>39</v>
@@ -1829,7 +1826,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51">
@@ -1840,7 +1837,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51">
@@ -1851,7 +1848,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="52" thickBot="1">
@@ -1862,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1890,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -1916,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="33.75" customHeight="1">
@@ -1924,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17">
@@ -1935,10 +1932,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33.75" customHeight="1">
@@ -1946,19 +1943,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="33.75" customHeight="1">
       <c r="A7" s="42"/>
       <c r="B7" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" thickBot="1">
@@ -1969,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1981,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1996,14 +1993,14 @@
   <sheetData>
     <row r="1" spans="1:4" s="22" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>3</v>
@@ -2020,69 +2017,69 @@
         <v>46</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>97</v>
-      </c>
       <c r="D3" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51">
       <c r="A4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>49</v>
-      </c>
       <c r="D4" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="153">
       <c r="A5" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="C5" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119">
       <c r="A6" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="C6" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="56" t="s">
-        <v>54</v>
-      </c>
       <c r="D6" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86" thickBot="1">
       <c r="A7" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2095,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2108,7 +2105,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -2123,128 +2120,128 @@
         <v>46</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34">
       <c r="A3" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="102">
       <c r="A4" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34">
       <c r="A5" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="52"/>
       <c r="F5" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136">
       <c r="A6" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34">
       <c r="A7" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="52"/>
       <c r="F7" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86" thickBot="1">
       <c r="A8" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2297,21 +2294,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008848E62C5F483F46BBC45A037BA06456" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9a231ef8203bd2df6f980a33ee7564c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="647e26e098842d3908dd56dced403b39" ns2:_="">
     <xsd:import namespace="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
@@ -2457,10 +2439,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3CD046-562E-4048-8CB3-7B082ACE1CD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2482,19 +2489,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3CD046-562E-4048-8CB3-7B082ACE1CD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Several small changes in some text.
</commit_message>
<xml_diff>
--- a/scoring_table.xlsx
+++ b/scoring_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/PycharmProjects/DeTTECT-private/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/VSCode/DeTTECT-private/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E722A-9C3E-5049-BD71-FEA725D581E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AFB856-AD15-034C-AA1B-A1427DD552A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detection scores - descriptions" sheetId="1" r:id="rId1"/>
@@ -173,12 +173,6 @@
     <t>Device completeness</t>
   </si>
   <si>
-    <t>Indicates to what degree the data has the required information/fields.</t>
-  </si>
-  <si>
-    <t>Are all the required data fields in the event present to perform my investigation?</t>
-  </si>
-  <si>
     <t>Timeliness</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>Indicates how long the data is stored compared to the desired data retention period.</t>
   </si>
   <si>
-    <t>Indicates if the required data is available for all involved devices.</t>
-  </si>
-  <si>
     <t>When doing a hunting investigation can we cover all devices/users that we need to?</t>
   </si>
   <si>
@@ -393,6 +384,15 @@
   </si>
   <si>
     <t>100% of the fields are standardized in name and type.</t>
+  </si>
+  <si>
+    <t>Indicates to what degree the data has the required information/fields, and to what degree those fields contain data.</t>
+  </si>
+  <si>
+    <t>Are all the required data fields in the event present and contain data to perform my investigation?</t>
+  </si>
+  <si>
+    <t>Indicates if the required data is available for all devices.</t>
   </si>
 </sst>
 </file>
@@ -895,7 +895,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1075,6 +1075,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1411,7 +1414,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1469,7 +1472,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="104" customHeight="1">
@@ -1620,7 +1623,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
@@ -1646,7 +1649,7 @@
         <v>24</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>25</v>
@@ -1672,10 +1675,10 @@
         <v>29</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>26</v>
@@ -1698,7 +1701,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>33</v>
@@ -1724,13 +1727,13 @@
         <v>32</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>37</v>
@@ -1750,13 +1753,13 @@
         <v>32</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>39</v>
@@ -1826,7 +1829,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51">
@@ -1837,7 +1840,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51">
@@ -1848,7 +1851,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="52" thickBot="1">
@@ -1859,7 +1862,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1890,7 +1893,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -1913,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="33.75" customHeight="1">
@@ -1921,10 +1924,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17">
@@ -1932,10 +1935,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33.75" customHeight="1">
@@ -1943,19 +1946,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="33.75" customHeight="1">
       <c r="A7" s="42"/>
       <c r="B7" s="47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" thickBot="1">
@@ -1966,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1978,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1993,14 +1996,14 @@
   <sheetData>
     <row r="1" spans="1:4" s="22" customFormat="1" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>3</v>
@@ -2016,70 +2019,70 @@
       <c r="A3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="29" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="85">
+      <c r="A4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="51">
-      <c r="A4" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="153">
       <c r="A5" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119">
       <c r="A6" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>53</v>
-      </c>
       <c r="D6" s="57" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86" thickBot="1">
       <c r="A7" s="58" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="59" t="s">
-        <v>97</v>
-      </c>
       <c r="D7" s="60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2092,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2105,7 +2108,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -2120,128 +2123,128 @@
         <v>46</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>51</v>
-      </c>
       <c r="F2" s="54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34">
       <c r="A3" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="102">
       <c r="A4" s="35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34">
       <c r="A5" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="52"/>
       <c r="F5" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136">
       <c r="A6" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34">
       <c r="A7" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="52"/>
       <c r="F7" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86" thickBot="1">
       <c r="A8" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2440,18 +2443,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2473,6 +2476,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2486,12 +2497,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed the colour for detection score 0 (forensics)
</commit_message>
<xml_diff>
--- a/scoring_table.xlsx
+++ b/scoring_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/VSCode/DeTTECT-private/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AFB856-AD15-034C-AA1B-A1427DD552A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE780008-248E-804C-9474-C5D538003DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="27940" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detection scores - descriptions" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,6 +562,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9C27B0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -895,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1079,6 +1085,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,6 +1097,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9C27B0"/>
       <color rgb="FF4A148C"/>
       <color rgb="FF7B1FA2"/>
       <color rgb="FFE1BEE7"/>
@@ -1097,7 +1107,6 @@
       <color rgb="FF27C34A"/>
       <color rgb="FF8BC38E"/>
       <color rgb="FF64B5F6"/>
-      <color rgb="FFDCEDC8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1413,8 +1422,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1457,7 +1466,7 @@
       <c r="A4" s="15">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="62" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1533,7 +1542,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1616,7 +1625,7 @@
       <c r="A4" s="15">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="62" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1981,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2297,6 +2306,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008848E62C5F483F46BBC45A037BA06456" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9a231ef8203bd2df6f980a33ee7564c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="647e26e098842d3908dd56dced403b39" ns2:_="">
     <xsd:import namespace="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
@@ -2442,22 +2466,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B3CD046-562E-4048-8CB3-7B082ACE1CD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2473,28 +2506,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE39A82-E2F5-4475-B886-1722EBC56E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC15240-37AB-4142-BAE6-7A699C18D81B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="52fa3a3b-9d90-4d6b-aa36-dcd226ed9483"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>